<commit_message>
Time Stamp added to the code
</commit_message>
<xml_diff>
--- a/Weather/src/newFile.xlsx
+++ b/Weather/src/newFile.xlsx
@@ -27,7 +27,10 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+  <si>
+    <t>Time Stamp</t>
+  </si>
   <si>
     <t>Temperature</t>
   </si>
@@ -39,6 +42,12 @@
   </si>
   <si>
     <t>Wind Speed</t>
+  </si>
+  <si>
+    <t>2017.05.19 16.07.33</t>
+  </si>
+  <si>
+    <t>2017.05.19 16.08.17</t>
   </si>
 </sst>
 </file>
@@ -354,7 +363,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E16" sqref="A1:XFD1048576"/>
@@ -375,63 +384,39 @@
       <c r="D1" t="s">
         <v>3</v>
       </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="2">
-      <c r="A2" t="n">
-        <v>301.19000244140625</v>
+      <c r="A2" t="s">
+        <v>5</v>
       </c>
       <c r="B2" t="n">
-        <v>32.0</v>
+        <v>301.0899963378906</v>
       </c>
       <c r="C2" t="n">
+        <v>30.0</v>
+      </c>
+      <c r="D2" t="n">
         <v>1012.0</v>
       </c>
-      <c r="D2" t="n">
-        <v>5.099999904632568</v>
-      </c>
     </row>
-    <row r="3"/>
-    <row r="4">
-      <c r="A4" t="n">
-        <v>301.19000244140625</v>
-      </c>
-      <c r="B4" t="n">
-        <v>32.0</v>
-      </c>
-      <c r="C4" t="n">
+    <row r="3">
+      <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" t="n">
+        <v>301.0899963378906</v>
+      </c>
+      <c r="C3" t="n">
+        <v>30.0</v>
+      </c>
+      <c r="D3" t="n">
         <v>1012.0</v>
       </c>
-      <c r="D4" t="n">
-        <v>5.099999904632568</v>
-      </c>
-    </row>
-    <row r="5"/>
-    <row r="6">
-      <c r="A6" t="n">
-        <v>301.19000244140625</v>
-      </c>
-      <c r="B6" t="n">
-        <v>32.0</v>
-      </c>
-      <c r="C6" t="n">
-        <v>1012.0</v>
-      </c>
-      <c r="D6" t="n">
-        <v>5.099999904632568</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="n">
-        <v>301.19000244140625</v>
-      </c>
-      <c r="B7" t="n">
-        <v>32.0</v>
-      </c>
-      <c r="C7" t="n">
-        <v>1012.0</v>
-      </c>
-      <c r="D7" t="n">
-        <v>5.099999904632568</v>
+      <c r="E3" t="n">
+        <v>4.599999904632568</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Code is added and the predicted temperature, pressure and humidity is getting displayed
</commit_message>
<xml_diff>
--- a/Weather/src/newFile.xlsx
+++ b/Weather/src/newFile.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>Time Stamp</t>
   </si>
@@ -48,6 +48,39 @@
   </si>
   <si>
     <t>2017.05.19 16.08.17</t>
+  </si>
+  <si>
+    <t>2017.05.20 13.39.32</t>
+  </si>
+  <si>
+    <t>2017.05.20 14.11.10</t>
+  </si>
+  <si>
+    <t>2017.05.20 14.14.51</t>
+  </si>
+  <si>
+    <t>2017.05.21 11.49.32</t>
+  </si>
+  <si>
+    <t>2017.05.21 12.18.31</t>
+  </si>
+  <si>
+    <t>2017.05.21 12.19.17</t>
+  </si>
+  <si>
+    <t>2017.05.21 12.22.03</t>
+  </si>
+  <si>
+    <t>2017.05.21 12.29.27</t>
+  </si>
+  <si>
+    <t>2017.05.21 12.32.26</t>
+  </si>
+  <si>
+    <t>2017.05.21 12.34.57</t>
+  </si>
+  <si>
+    <t>2017.05.21 12.45.55</t>
   </si>
 </sst>
 </file>
@@ -363,7 +396,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:F14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E16" sqref="A1:XFD1048576"/>
@@ -419,6 +452,193 @@
         <v>4.599999904632568</v>
       </c>
     </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" t="n">
+        <v>304.8999938964844</v>
+      </c>
+      <c r="C4" t="n">
+        <v>25.0</v>
+      </c>
+      <c r="D4" t="n">
+        <v>1011.0</v>
+      </c>
+      <c r="E4" t="n">
+        <v>5.099999904632568</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" t="n">
+        <v>304.8900146484375</v>
+      </c>
+      <c r="C5" t="n">
+        <v>25.0</v>
+      </c>
+      <c r="D5" t="n">
+        <v>1011.0</v>
+      </c>
+      <c r="E5" t="n">
+        <v>5.099999904632568</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" t="n">
+        <v>31.15999984741211</v>
+      </c>
+      <c r="C6" t="n">
+        <v>26.0</v>
+      </c>
+      <c r="D6" t="n">
+        <v>1011.0</v>
+      </c>
+      <c r="E6" t="n">
+        <v>4.599999904632568</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" t="n">
+        <v>27.0</v>
+      </c>
+      <c r="C7" t="n">
+        <v>57.0</v>
+      </c>
+      <c r="D7" t="n">
+        <v>1013.0</v>
+      </c>
+      <c r="E7" t="n">
+        <v>3.0999999046325684</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8" t="n">
+        <v>27.829999923706055</v>
+      </c>
+      <c r="C8" t="n">
+        <v>47.0</v>
+      </c>
+      <c r="D8" t="n">
+        <v>1013.0</v>
+      </c>
+      <c r="E8" t="n">
+        <v>4.599999904632568</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9" t="n">
+        <v>27.829999923706055</v>
+      </c>
+      <c r="C9" t="n">
+        <v>47.0</v>
+      </c>
+      <c r="D9" t="n">
+        <v>1013.0</v>
+      </c>
+      <c r="E9" t="n">
+        <v>4.599999904632568</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="s">
+        <v>13</v>
+      </c>
+      <c r="B10" t="n">
+        <v>27.829999923706055</v>
+      </c>
+      <c r="C10" t="n">
+        <v>47.0</v>
+      </c>
+      <c r="D10" t="n">
+        <v>1013.0</v>
+      </c>
+      <c r="E10" t="n">
+        <v>4.599999904632568</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="s">
+        <v>14</v>
+      </c>
+      <c r="B11" t="n">
+        <v>27.829999923706055</v>
+      </c>
+      <c r="C11" t="n">
+        <v>47.0</v>
+      </c>
+      <c r="D11" t="n">
+        <v>1013.0</v>
+      </c>
+      <c r="E11" t="n">
+        <v>4.599999904632568</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="s">
+        <v>15</v>
+      </c>
+      <c r="B12" t="n">
+        <v>27.829999923706055</v>
+      </c>
+      <c r="C12" t="n">
+        <v>47.0</v>
+      </c>
+      <c r="D12" t="n">
+        <v>1013.0</v>
+      </c>
+      <c r="E12" t="n">
+        <v>4.599999904632568</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="s">
+        <v>16</v>
+      </c>
+      <c r="B13" t="n">
+        <v>27.829999923706055</v>
+      </c>
+      <c r="C13" t="n">
+        <v>47.0</v>
+      </c>
+      <c r="D13" t="n">
+        <v>1013.0</v>
+      </c>
+      <c r="E13" t="n">
+        <v>4.599999904632568</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="s">
+        <v>17</v>
+      </c>
+      <c r="B14" t="n">
+        <v>27.829999923706055</v>
+      </c>
+      <c r="C14" t="n">
+        <v>47.0</v>
+      </c>
+      <c r="D14" t="n">
+        <v>1013.0</v>
+      </c>
+      <c r="E14" t="n">
+        <v>4.599999904632568</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>

<commit_message>
Date from and to of forecast has to be added. Rest all is working fine and the data is getting saved in the database file
</commit_message>
<xml_diff>
--- a/Weather/src/newFile.xlsx
+++ b/Weather/src/newFile.xlsx
@@ -27,60 +27,51 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="15">
   <si>
     <t>Time Stamp</t>
   </si>
   <si>
-    <t>Temperature</t>
-  </si>
-  <si>
-    <t>Humidity</t>
-  </si>
-  <si>
-    <t>Pressure</t>
-  </si>
-  <si>
-    <t>Wind Speed</t>
-  </si>
-  <si>
-    <t>2017.05.19 16.07.33</t>
-  </si>
-  <si>
-    <t>2017.05.19 16.08.17</t>
-  </si>
-  <si>
-    <t>2017.05.20 13.39.32</t>
-  </si>
-  <si>
-    <t>2017.05.20 14.11.10</t>
-  </si>
-  <si>
-    <t>2017.05.20 14.14.51</t>
-  </si>
-  <si>
-    <t>2017.05.21 11.49.32</t>
-  </si>
-  <si>
-    <t>2017.05.21 12.18.31</t>
-  </si>
-  <si>
-    <t>2017.05.21 12.19.17</t>
-  </si>
-  <si>
-    <t>2017.05.21 12.22.03</t>
-  </si>
-  <si>
-    <t>2017.05.21 12.29.27</t>
-  </si>
-  <si>
-    <t>2017.05.21 12.32.26</t>
-  </si>
-  <si>
-    <t>2017.05.21 12.34.57</t>
-  </si>
-  <si>
-    <t>2017.05.21 12.45.55</t>
+    <t>Temperature (celcius)</t>
+  </si>
+  <si>
+    <t>Humidity (%)</t>
+  </si>
+  <si>
+    <t>Pressure (hPa)</t>
+  </si>
+  <si>
+    <t>Wind Speed (mps)</t>
+  </si>
+  <si>
+    <t>Forecasted Temperature (celcius)</t>
+  </si>
+  <si>
+    <t>Forecasted HUmidity (%)</t>
+  </si>
+  <si>
+    <t>Forecasted Pressure (hPa)</t>
+  </si>
+  <si>
+    <t>Forecasted Precipitation</t>
+  </si>
+  <si>
+    <t>Forecasted Wind Speed (mps)</t>
+  </si>
+  <si>
+    <t>2017.05.21 14.48.46</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>2017.05.21 14.58.13</t>
+  </si>
+  <si>
+    <t>2017.05.21 15.07.19</t>
+  </si>
+  <si>
+    <t>2017.05.21 15.08.20</t>
   </si>
 </sst>
 </file>
@@ -396,13 +387,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F14"/>
+  <dimension ref="A1:K5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E16" sqref="A1:XFD1048576"/>
+      <selection activeCell="F12" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="17.6640625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="12.1640625" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="8.5" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="8.1640625" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="12.1640625" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="21.1640625" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="18.1640625" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="17.5" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="20.83203125" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="20.33203125" collapsed="true"/>
+  </cols>
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
@@ -420,223 +423,148 @@
       <c r="E1" t="s">
         <v>4</v>
       </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="B2" t="n">
-        <v>301.0899963378906</v>
+        <v>28.530000686645508</v>
       </c>
       <c r="C2" t="n">
+        <v>47.0</v>
+      </c>
+      <c r="D2" t="n">
+        <v>1013.0</v>
+      </c>
+      <c r="E2" t="n">
+        <v>3.5999999046325684</v>
+      </c>
+      <c r="F2" t="n">
+        <v>29.170000076293945</v>
+      </c>
+      <c r="G2" t="n">
+        <v>994.510009765625</v>
+      </c>
+      <c r="H2" t="n">
         <v>30.0</v>
       </c>
-      <c r="D2" t="n">
-        <v>1012.0</v>
+      <c r="I2" t="s">
+        <v>11</v>
+      </c>
+      <c r="J2" t="n">
+        <v>2.359999895095825</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="B3" t="n">
-        <v>301.0899963378906</v>
+        <v>28.530000686645508</v>
       </c>
       <c r="C3" t="n">
+        <v>47.0</v>
+      </c>
+      <c r="D3" t="n">
+        <v>1013.0</v>
+      </c>
+      <c r="E3" t="n">
+        <v>3.5999999046325684</v>
+      </c>
+      <c r="F3" t="n">
+        <v>29.170000076293945</v>
+      </c>
+      <c r="G3" t="n">
+        <v>994.510009765625</v>
+      </c>
+      <c r="H3" t="n">
         <v>30.0</v>
       </c>
-      <c r="D3" t="n">
-        <v>1012.0</v>
-      </c>
-      <c r="E3" t="n">
-        <v>4.599999904632568</v>
+      <c r="I3" t="s">
+        <v>11</v>
+      </c>
+      <c r="J3" t="n">
+        <v>2.359999895095825</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="B4" t="n">
-        <v>304.8999938964844</v>
+        <v>28.530000686645508</v>
       </c>
       <c r="C4" t="n">
-        <v>25.0</v>
+        <v>47.0</v>
       </c>
       <c r="D4" t="n">
-        <v>1011.0</v>
+        <v>1013.0</v>
       </c>
       <c r="E4" t="n">
-        <v>5.099999904632568</v>
+        <v>3.5999999046325684</v>
+      </c>
+      <c r="F4" t="n">
+        <v>29.170000076293945</v>
+      </c>
+      <c r="G4" t="n">
+        <v>994.510009765625</v>
+      </c>
+      <c r="H4" t="n">
+        <v>30.0</v>
+      </c>
+      <c r="I4" t="s">
+        <v>11</v>
+      </c>
+      <c r="J4" t="n">
+        <v>2.359999895095825</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="B5" t="n">
-        <v>304.8900146484375</v>
+        <v>28.530000686645508</v>
       </c>
       <c r="C5" t="n">
-        <v>25.0</v>
+        <v>47.0</v>
       </c>
       <c r="D5" t="n">
-        <v>1011.0</v>
+        <v>1013.0</v>
       </c>
       <c r="E5" t="n">
-        <v>5.099999904632568</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="s">
-        <v>9</v>
-      </c>
-      <c r="B6" t="n">
-        <v>31.15999984741211</v>
-      </c>
-      <c r="C6" t="n">
-        <v>26.0</v>
-      </c>
-      <c r="D6" t="n">
-        <v>1011.0</v>
-      </c>
-      <c r="E6" t="n">
-        <v>4.599999904632568</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="s">
-        <v>10</v>
-      </c>
-      <c r="B7" t="n">
-        <v>27.0</v>
-      </c>
-      <c r="C7" t="n">
-        <v>57.0</v>
-      </c>
-      <c r="D7" t="n">
-        <v>1013.0</v>
-      </c>
-      <c r="E7" t="n">
-        <v>3.0999999046325684</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="s">
+        <v>3.5999999046325684</v>
+      </c>
+      <c r="F5" t="n">
+        <v>29.170000076293945</v>
+      </c>
+      <c r="G5" t="n">
+        <v>994.510009765625</v>
+      </c>
+      <c r="H5" t="n">
+        <v>30.0</v>
+      </c>
+      <c r="I5" t="s">
         <v>11</v>
       </c>
-      <c r="B8" t="n">
-        <v>27.829999923706055</v>
-      </c>
-      <c r="C8" t="n">
-        <v>47.0</v>
-      </c>
-      <c r="D8" t="n">
-        <v>1013.0</v>
-      </c>
-      <c r="E8" t="n">
-        <v>4.599999904632568</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="s">
-        <v>12</v>
-      </c>
-      <c r="B9" t="n">
-        <v>27.829999923706055</v>
-      </c>
-      <c r="C9" t="n">
-        <v>47.0</v>
-      </c>
-      <c r="D9" t="n">
-        <v>1013.0</v>
-      </c>
-      <c r="E9" t="n">
-        <v>4.599999904632568</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="s">
-        <v>13</v>
-      </c>
-      <c r="B10" t="n">
-        <v>27.829999923706055</v>
-      </c>
-      <c r="C10" t="n">
-        <v>47.0</v>
-      </c>
-      <c r="D10" t="n">
-        <v>1013.0</v>
-      </c>
-      <c r="E10" t="n">
-        <v>4.599999904632568</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="s">
-        <v>14</v>
-      </c>
-      <c r="B11" t="n">
-        <v>27.829999923706055</v>
-      </c>
-      <c r="C11" t="n">
-        <v>47.0</v>
-      </c>
-      <c r="D11" t="n">
-        <v>1013.0</v>
-      </c>
-      <c r="E11" t="n">
-        <v>4.599999904632568</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="s">
-        <v>15</v>
-      </c>
-      <c r="B12" t="n">
-        <v>27.829999923706055</v>
-      </c>
-      <c r="C12" t="n">
-        <v>47.0</v>
-      </c>
-      <c r="D12" t="n">
-        <v>1013.0</v>
-      </c>
-      <c r="E12" t="n">
-        <v>4.599999904632568</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="s">
-        <v>16</v>
-      </c>
-      <c r="B13" t="n">
-        <v>27.829999923706055</v>
-      </c>
-      <c r="C13" t="n">
-        <v>47.0</v>
-      </c>
-      <c r="D13" t="n">
-        <v>1013.0</v>
-      </c>
-      <c r="E13" t="n">
-        <v>4.599999904632568</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="s">
-        <v>17</v>
-      </c>
-      <c r="B14" t="n">
-        <v>27.829999923706055</v>
-      </c>
-      <c r="C14" t="n">
-        <v>47.0</v>
-      </c>
-      <c r="D14" t="n">
-        <v>1013.0</v>
-      </c>
-      <c r="E14" t="n">
-        <v>4.599999904632568</v>
+      <c r="J5" t="n">
+        <v>2.359999895095825</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
All the forecasted data along with time is updated in the excel file
</commit_message>
<xml_diff>
--- a/Weather/src/newFile.xlsx
+++ b/Weather/src/newFile.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="20">
   <si>
     <t>Time Stamp</t>
   </si>
@@ -44,13 +44,19 @@
     <t>Wind Speed (mps)</t>
   </si>
   <si>
+    <t>Forecasted Time ( From )</t>
+  </si>
+  <si>
+    <t>Forecasted Time ( To )</t>
+  </si>
+  <si>
     <t>Forecasted Temperature (celcius)</t>
   </si>
   <si>
-    <t>Forecasted HUmidity (%)</t>
-  </si>
-  <si>
-    <t>Forecasted Pressure (hPa)</t>
+    <t>Forecasted Pressure (hPa))</t>
+  </si>
+  <si>
+    <t>Forecasted Humidity (%</t>
   </si>
   <si>
     <t>Forecasted Precipitation</t>
@@ -59,19 +65,28 @@
     <t>Forecasted Wind Speed (mps)</t>
   </si>
   <si>
-    <t>2017.05.21 14.48.46</t>
+    <t>2017.05.21 15.49.52</t>
+  </si>
+  <si>
+    <t>2017-05-21T21:00:00</t>
+  </si>
+  <si>
+    <t>2017-05-22T00:00:00</t>
   </si>
   <si>
     <t/>
   </si>
   <si>
-    <t>2017.05.21 14.58.13</t>
-  </si>
-  <si>
-    <t>2017.05.21 15.07.19</t>
-  </si>
-  <si>
-    <t>2017.05.21 15.08.20</t>
+    <t>2017.05.21 15.50.42</t>
+  </si>
+  <si>
+    <t>2017.05.21 15.51.20</t>
+  </si>
+  <si>
+    <t>2017.05.21 15.51.27</t>
+  </si>
+  <si>
+    <t>2017.05.21 15.51.35</t>
   </si>
 </sst>
 </file>
@@ -387,24 +402,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K5"/>
+  <dimension ref="A1:M6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F12" sqref="A1:XFD1048576"/>
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" bestFit="true" customWidth="true" width="17.6640625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="12.1640625" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="8.5" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="8.1640625" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="12.1640625" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="21.1640625" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="18.1640625" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="17.5" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="18.83203125" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="11.6640625" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="12.83203125" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="19.1640625" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="28.33203125" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="22.83203125" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="20.5" collapsed="true"/>
     <col min="9" max="9" bestFit="true" customWidth="true" width="20.83203125" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" width="20.33203125" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="25.33203125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -438,132 +453,194 @@
       <c r="J1" t="s">
         <v>9</v>
       </c>
+      <c r="K1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B2" t="n">
-        <v>28.530000686645508</v>
+        <v>28.770000457763672</v>
       </c>
       <c r="C2" t="n">
-        <v>47.0</v>
+        <v>44.0</v>
       </c>
       <c r="D2" t="n">
         <v>1013.0</v>
       </c>
       <c r="E2" t="n">
-        <v>3.5999999046325684</v>
-      </c>
-      <c r="F2" t="n">
-        <v>29.170000076293945</v>
-      </c>
-      <c r="G2" t="n">
+        <v>4.599999904632568</v>
+      </c>
+      <c r="F2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H2" t="n">
+        <v>27.84000015258789</v>
+      </c>
+      <c r="I2" t="n">
         <v>994.510009765625</v>
       </c>
-      <c r="H2" t="n">
+      <c r="J2" t="n">
         <v>30.0</v>
       </c>
-      <c r="I2" t="s">
-        <v>11</v>
-      </c>
-      <c r="J2" t="n">
-        <v>2.359999895095825</v>
+      <c r="K2" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="B3" t="n">
-        <v>28.530000686645508</v>
+        <v>28.770000457763672</v>
       </c>
       <c r="C3" t="n">
-        <v>47.0</v>
+        <v>44.0</v>
       </c>
       <c r="D3" t="n">
         <v>1013.0</v>
       </c>
       <c r="E3" t="n">
-        <v>3.5999999046325684</v>
-      </c>
-      <c r="F3" t="n">
-        <v>29.170000076293945</v>
-      </c>
-      <c r="G3" t="n">
+        <v>4.599999904632568</v>
+      </c>
+      <c r="F3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G3" t="s">
+        <v>14</v>
+      </c>
+      <c r="H3" t="n">
+        <v>27.84000015258789</v>
+      </c>
+      <c r="I3" t="n">
         <v>994.510009765625</v>
       </c>
-      <c r="H3" t="n">
+      <c r="J3" t="n">
         <v>30.0</v>
       </c>
-      <c r="I3" t="s">
-        <v>11</v>
-      </c>
-      <c r="J3" t="n">
-        <v>2.359999895095825</v>
+      <c r="K3" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="B4" t="n">
-        <v>28.530000686645508</v>
+        <v>28.770000457763672</v>
       </c>
       <c r="C4" t="n">
-        <v>47.0</v>
+        <v>44.0</v>
       </c>
       <c r="D4" t="n">
         <v>1013.0</v>
       </c>
       <c r="E4" t="n">
-        <v>3.5999999046325684</v>
-      </c>
-      <c r="F4" t="n">
-        <v>29.170000076293945</v>
-      </c>
-      <c r="G4" t="n">
+        <v>4.599999904632568</v>
+      </c>
+      <c r="F4" t="s">
+        <v>13</v>
+      </c>
+      <c r="G4" t="s">
+        <v>14</v>
+      </c>
+      <c r="H4" t="n">
+        <v>27.84000015258789</v>
+      </c>
+      <c r="I4" t="n">
         <v>994.510009765625</v>
       </c>
-      <c r="H4" t="n">
+      <c r="J4" t="n">
         <v>30.0</v>
       </c>
-      <c r="I4" t="s">
-        <v>11</v>
-      </c>
-      <c r="J4" t="n">
+      <c r="K4" t="s">
+        <v>15</v>
+      </c>
+      <c r="L4" t="n">
         <v>2.359999895095825</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="B5" t="n">
-        <v>28.530000686645508</v>
+        <v>28.770000457763672</v>
       </c>
       <c r="C5" t="n">
-        <v>47.0</v>
+        <v>44.0</v>
       </c>
       <c r="D5" t="n">
         <v>1013.0</v>
       </c>
       <c r="E5" t="n">
-        <v>3.5999999046325684</v>
-      </c>
-      <c r="F5" t="n">
-        <v>29.170000076293945</v>
-      </c>
-      <c r="G5" t="n">
+        <v>4.599999904632568</v>
+      </c>
+      <c r="F5" t="s">
+        <v>13</v>
+      </c>
+      <c r="G5" t="s">
+        <v>14</v>
+      </c>
+      <c r="H5" t="n">
+        <v>27.84000015258789</v>
+      </c>
+      <c r="I5" t="n">
         <v>994.510009765625</v>
       </c>
-      <c r="H5" t="n">
+      <c r="J5" t="n">
         <v>30.0</v>
       </c>
-      <c r="I5" t="s">
-        <v>11</v>
-      </c>
-      <c r="J5" t="n">
+      <c r="K5" t="s">
+        <v>15</v>
+      </c>
+      <c r="L5" t="n">
+        <v>2.359999895095825</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6" t="n">
+        <v>28.770000457763672</v>
+      </c>
+      <c r="C6" t="n">
+        <v>44.0</v>
+      </c>
+      <c r="D6" t="n">
+        <v>1013.0</v>
+      </c>
+      <c r="E6" t="n">
+        <v>4.599999904632568</v>
+      </c>
+      <c r="F6" t="s">
+        <v>13</v>
+      </c>
+      <c r="G6" t="s">
+        <v>14</v>
+      </c>
+      <c r="H6" t="n">
+        <v>27.84000015258789</v>
+      </c>
+      <c r="I6" t="n">
+        <v>994.510009765625</v>
+      </c>
+      <c r="J6" t="n">
+        <v>30.0</v>
+      </c>
+      <c r="K6" t="s">
+        <v>15</v>
+      </c>
+      <c r="L6" t="n">
         <v>2.359999895095825</v>
       </c>
     </row>

</xml_diff>